<commit_message>
++ update code import, fix bug
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/CommercialCustomerImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/CommercialCustomerImportTemplate.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.an\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,68 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
-  <si>
-    <t>Contact Person</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Zipcode</t>
   </si>
   <si>
-    <t xml:space="preserve">Email </t>
-  </si>
-  <si>
-    <t>Partners Bank Account</t>
-  </si>
-  <si>
-    <t>Bank Name</t>
-  </si>
-  <si>
-    <t>Swift Code</t>
-  </si>
-  <si>
-    <t>Bank Address</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>ABC</t>
   </si>
   <si>
-    <t>Name Abr(*)</t>
-  </si>
-  <si>
-    <t>Name EN(*)</t>
-  </si>
-  <si>
-    <t>Name Local(*)</t>
-  </si>
-  <si>
     <t>Taxcode(*)</t>
   </si>
   <si>
-    <t>Billing  Address EN(*)</t>
-  </si>
-  <si>
-    <t>Billing Address Local(*)</t>
-  </si>
-  <si>
-    <t>Shipping Address Local(*)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> City </t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Shipping  Address EN</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -129,56 +78,86 @@
     <t>Viet Nam</t>
   </si>
   <si>
-    <t>Bac Giang</t>
-  </si>
-  <si>
-    <t>Fax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country </t>
-  </si>
-  <si>
     <t>Internal Reference</t>
   </si>
   <si>
     <t>Paynment Metho</t>
   </si>
   <si>
-    <t>Salesman Default</t>
-  </si>
-  <si>
-    <t>A/C Reference</t>
-  </si>
-  <si>
     <t>Billing Phone</t>
   </si>
   <si>
     <t>Billing Email</t>
   </si>
   <si>
-    <t>an@gmail.com</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>bankno</t>
-  </si>
-  <si>
-    <t>bankname</t>
-  </si>
-  <si>
     <t>ABCDEF</t>
   </si>
   <si>
-    <t>0100103224</t>
+    <t>Name ABBR (*)</t>
+  </si>
+  <si>
+    <t>English Name (*)</t>
+  </si>
+  <si>
+    <t>Local Name (*)</t>
+  </si>
+  <si>
+    <t>Partner Location (*)</t>
+  </si>
+  <si>
+    <t>Domestic</t>
+  </si>
+  <si>
+    <t>A/C Referrence</t>
+  </si>
+  <si>
+    <t>Shipping Address EN (*)</t>
+  </si>
+  <si>
+    <t>Shipping Address Local (*)</t>
+  </si>
+  <si>
+    <t>Country (*)</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Billing Address EN (*)</t>
+  </si>
+  <si>
+    <t>Billing Address Local (*)</t>
+  </si>
+  <si>
+    <t>Nghe An</t>
+  </si>
+  <si>
+    <t>Person Contact</t>
+  </si>
+  <si>
+    <t>Contact Phone Number</t>
+  </si>
+  <si>
+    <t>Fax No</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work Phone </t>
+  </si>
+  <si>
+    <t>Shipping Address EN</t>
+  </si>
+  <si>
+    <t>Shipping Address Local</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,21 +172,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -234,30 +217,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,207 +534,159 @@
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="37.5703125" customWidth="1"/>
-    <col min="15" max="15" width="28.5703125" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" customWidth="1"/>
-    <col min="17" max="17" width="16.5703125" customWidth="1"/>
-    <col min="20" max="21" width="17.85546875" customWidth="1"/>
-    <col min="22" max="22" width="25.42578125" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="37.5703125" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" customWidth="1"/>
+    <col min="19" max="24" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="U1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1">
         <v>3123123190</v>
-      </c>
-      <c r="E2" s="1">
-        <v>123</v>
       </c>
       <c r="F2" s="1">
         <v>123</v>
       </c>
-      <c r="G2" s="1">
-        <v>123</v>
-      </c>
-      <c r="H2" s="1">
-        <v>23</v>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="1">
-        <v>143223</v>
-      </c>
-      <c r="N2" s="1">
-        <v>54353123</v>
-      </c>
-      <c r="O2" s="1">
-        <v>433</v>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="1">
-        <v>13445</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="X2" s="4">
-        <v>123</v>
-      </c>
-      <c r="Y2" s="4">
-        <v>123</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>123</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>2525</v>
-      </c>
-      <c r="AB2" s="4">
-        <v>2525</v>
-      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1"/>
-  </hyperlinks>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+      <formula1>"Domestic,Oversea"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -763,66 +702,66 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>